<commit_message>
Bulk upload transfer auto cost done
</commit_message>
<xml_diff>
--- a/functions/templates/Line Transfer.xlsx
+++ b/functions/templates/Line Transfer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="124">
   <si>
     <t xml:space="preserve">ID Number </t>
   </si>
@@ -33,7 +33,7 @@
     <t>Sub Section</t>
   </si>
   <si>
-    <t>Production 1</t>
+    <t>PROD</t>
   </si>
   <si>
     <t>Section 2</t>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Daihatsu Final</t>
-  </si>
-  <si>
-    <t>Production 2</t>
   </si>
   <si>
     <t>Section 5</t>
@@ -770,7 +767,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D239"/>
+  <dimension ref="A1:D241"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A155" sqref="A155"/>
@@ -1473,13 +1470,13 @@
         <v>3006</v>
       </c>
       <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
         <v>13</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>14</v>
-      </c>
-      <c r="D50" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1487,13 +1484,13 @@
         <v>3018</v>
       </c>
       <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
         <v>13</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>14</v>
-      </c>
-      <c r="D51" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1501,13 +1498,13 @@
         <v>3020</v>
       </c>
       <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
         <v>13</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>14</v>
-      </c>
-      <c r="D52" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1515,13 +1512,13 @@
         <v>3021</v>
       </c>
       <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
         <v>13</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>14</v>
-      </c>
-      <c r="D53" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1529,13 +1526,13 @@
         <v>3031</v>
       </c>
       <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
         <v>13</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>14</v>
-      </c>
-      <c r="D54" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1543,13 +1540,13 @@
         <v>3032</v>
       </c>
       <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
         <v>13</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>14</v>
-      </c>
-      <c r="D55" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1557,13 +1554,13 @@
         <v>3037</v>
       </c>
       <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
         <v>13</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>14</v>
-      </c>
-      <c r="D56" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1571,13 +1568,13 @@
         <v>3043</v>
       </c>
       <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
         <v>13</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>14</v>
-      </c>
-      <c r="D57" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1585,13 +1582,13 @@
         <v>3107</v>
       </c>
       <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
         <v>13</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>14</v>
-      </c>
-      <c r="D58" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1599,13 +1596,13 @@
         <v>3108</v>
       </c>
       <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
         <v>13</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>14</v>
-      </c>
-      <c r="D59" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1613,13 +1610,13 @@
         <v>3109</v>
       </c>
       <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
         <v>13</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>14</v>
-      </c>
-      <c r="D60" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1627,13 +1624,13 @@
         <v>3114</v>
       </c>
       <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
         <v>13</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>14</v>
-      </c>
-      <c r="D61" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1641,13 +1638,13 @@
         <v>3115</v>
       </c>
       <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
         <v>13</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>14</v>
-      </c>
-      <c r="D62" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1655,13 +1652,13 @@
         <v>3116</v>
       </c>
       <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
         <v>13</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>14</v>
-      </c>
-      <c r="D63" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1669,13 +1666,13 @@
         <v>3119</v>
       </c>
       <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
         <v>13</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>14</v>
-      </c>
-      <c r="D64" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1683,13 +1680,13 @@
         <v>3122</v>
       </c>
       <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
         <v>13</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>14</v>
-      </c>
-      <c r="D65" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1697,13 +1694,13 @@
         <v>3123</v>
       </c>
       <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
         <v>13</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>14</v>
-      </c>
-      <c r="D66" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1711,13 +1708,13 @@
         <v>3124</v>
       </c>
       <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
         <v>13</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>14</v>
-      </c>
-      <c r="D67" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1725,13 +1722,13 @@
         <v>3125</v>
       </c>
       <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
         <v>13</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>14</v>
-      </c>
-      <c r="D68" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1739,13 +1736,13 @@
         <v>3126</v>
       </c>
       <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
         <v>13</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>14</v>
-      </c>
-      <c r="D69" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1753,13 +1750,13 @@
         <v>3127</v>
       </c>
       <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
         <v>13</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>14</v>
-      </c>
-      <c r="D70" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1767,13 +1764,13 @@
         <v>3128</v>
       </c>
       <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
         <v>13</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>14</v>
-      </c>
-      <c r="D71" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1781,13 +1778,13 @@
         <v>3129</v>
       </c>
       <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
         <v>13</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>14</v>
-      </c>
-      <c r="D72" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1795,13 +1792,13 @@
         <v>3130</v>
       </c>
       <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
         <v>13</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>14</v>
-      </c>
-      <c r="D73" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1809,13 +1806,13 @@
         <v>3133</v>
       </c>
       <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
         <v>13</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>14</v>
-      </c>
-      <c r="D74" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1823,13 +1820,13 @@
         <v>3134</v>
       </c>
       <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
         <v>13</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>14</v>
-      </c>
-      <c r="D75" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1837,13 +1834,13 @@
         <v>3135</v>
       </c>
       <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
         <v>13</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>14</v>
-      </c>
-      <c r="D76" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1851,13 +1848,13 @@
         <v>3136</v>
       </c>
       <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
         <v>13</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>14</v>
-      </c>
-      <c r="D77" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1865,13 +1862,13 @@
         <v>3138</v>
       </c>
       <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
         <v>13</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>14</v>
-      </c>
-      <c r="D78" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1879,13 +1876,13 @@
         <v>3139</v>
       </c>
       <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
         <v>13</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>14</v>
-      </c>
-      <c r="D79" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1893,13 +1890,13 @@
         <v>3140</v>
       </c>
       <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
         <v>13</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>14</v>
-      </c>
-      <c r="D80" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1907,13 +1904,13 @@
         <v>3141</v>
       </c>
       <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
         <v>13</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>14</v>
-      </c>
-      <c r="D81" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1921,13 +1918,13 @@
         <v>3142</v>
       </c>
       <c r="B82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
         <v>13</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>14</v>
-      </c>
-      <c r="D82" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1941,7 +1938,7 @@
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1955,7 +1952,7 @@
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1969,7 +1966,7 @@
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1983,7 +1980,7 @@
         <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1997,7 +1994,7 @@
         <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2011,7 +2008,7 @@
         <v>6</v>
       </c>
       <c r="D88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2025,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2036,10 +2033,10 @@
         <v>5</v>
       </c>
       <c r="C90" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" t="s">
         <v>17</v>
-      </c>
-      <c r="D90" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2050,10 +2047,10 @@
         <v>5</v>
       </c>
       <c r="C91" t="s">
+        <v>16</v>
+      </c>
+      <c r="D91" t="s">
         <v>17</v>
-      </c>
-      <c r="D91" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2064,10 +2061,10 @@
         <v>5</v>
       </c>
       <c r="C92" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" t="s">
         <v>17</v>
-      </c>
-      <c r="D92" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2078,10 +2075,10 @@
         <v>5</v>
       </c>
       <c r="C93" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" t="s">
         <v>17</v>
-      </c>
-      <c r="D93" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2092,10 +2089,10 @@
         <v>5</v>
       </c>
       <c r="C94" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" t="s">
         <v>17</v>
-      </c>
-      <c r="D94" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2106,10 +2103,10 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" t="s">
         <v>17</v>
-      </c>
-      <c r="D95" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2120,10 +2117,10 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" t="s">
         <v>17</v>
-      </c>
-      <c r="D96" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2134,10 +2131,10 @@
         <v>5</v>
       </c>
       <c r="C97" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97" t="s">
         <v>17</v>
-      </c>
-      <c r="D97" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2148,10 +2145,10 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" t="s">
         <v>17</v>
-      </c>
-      <c r="D98" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2162,10 +2159,10 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" t="s">
         <v>17</v>
-      </c>
-      <c r="D99" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2176,10 +2173,10 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" t="s">
         <v>17</v>
-      </c>
-      <c r="D100" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2190,10 +2187,10 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101" t="s">
         <v>17</v>
-      </c>
-      <c r="D101" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2204,10 +2201,10 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" t="s">
         <v>17</v>
-      </c>
-      <c r="D102" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2218,10 +2215,10 @@
         <v>5</v>
       </c>
       <c r="C103" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103" t="s">
         <v>17</v>
-      </c>
-      <c r="D103" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2232,10 +2229,10 @@
         <v>5</v>
       </c>
       <c r="C104" t="s">
+        <v>16</v>
+      </c>
+      <c r="D104" t="s">
         <v>17</v>
-      </c>
-      <c r="D104" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2246,10 +2243,10 @@
         <v>5</v>
       </c>
       <c r="C105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" t="s">
         <v>17</v>
-      </c>
-      <c r="D105" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2260,10 +2257,10 @@
         <v>5</v>
       </c>
       <c r="C106" t="s">
+        <v>16</v>
+      </c>
+      <c r="D106" t="s">
         <v>17</v>
-      </c>
-      <c r="D106" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2274,10 +2271,10 @@
         <v>5</v>
       </c>
       <c r="C107" t="s">
+        <v>16</v>
+      </c>
+      <c r="D107" t="s">
         <v>17</v>
-      </c>
-      <c r="D107" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2288,10 +2285,10 @@
         <v>5</v>
       </c>
       <c r="C108" t="s">
+        <v>16</v>
+      </c>
+      <c r="D108" t="s">
         <v>17</v>
-      </c>
-      <c r="D108" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2302,10 +2299,10 @@
         <v>5</v>
       </c>
       <c r="C109" t="s">
+        <v>16</v>
+      </c>
+      <c r="D109" t="s">
         <v>17</v>
-      </c>
-      <c r="D109" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2316,10 +2313,10 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
+        <v>16</v>
+      </c>
+      <c r="D110" t="s">
         <v>17</v>
-      </c>
-      <c r="D110" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2330,10 +2327,10 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
+        <v>16</v>
+      </c>
+      <c r="D111" t="s">
         <v>17</v>
-      </c>
-      <c r="D111" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2344,10 +2341,10 @@
         <v>5</v>
       </c>
       <c r="C112" t="s">
+        <v>16</v>
+      </c>
+      <c r="D112" t="s">
         <v>17</v>
-      </c>
-      <c r="D112" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2358,10 +2355,10 @@
         <v>5</v>
       </c>
       <c r="C113" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113" t="s">
         <v>17</v>
-      </c>
-      <c r="D113" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2372,10 +2369,10 @@
         <v>5</v>
       </c>
       <c r="C114" t="s">
+        <v>16</v>
+      </c>
+      <c r="D114" t="s">
         <v>17</v>
-      </c>
-      <c r="D114" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2386,10 +2383,10 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
+        <v>16</v>
+      </c>
+      <c r="D115" t="s">
         <v>17</v>
-      </c>
-      <c r="D115" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2400,10 +2397,10 @@
         <v>5</v>
       </c>
       <c r="C116" t="s">
+        <v>16</v>
+      </c>
+      <c r="D116" t="s">
         <v>17</v>
-      </c>
-      <c r="D116" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2414,10 +2411,10 @@
         <v>5</v>
       </c>
       <c r="C117" t="s">
+        <v>16</v>
+      </c>
+      <c r="D117" t="s">
         <v>17</v>
-      </c>
-      <c r="D117" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2428,10 +2425,10 @@
         <v>5</v>
       </c>
       <c r="C118" t="s">
+        <v>16</v>
+      </c>
+      <c r="D118" t="s">
         <v>17</v>
-      </c>
-      <c r="D118" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2442,10 +2439,10 @@
         <v>5</v>
       </c>
       <c r="C119" t="s">
+        <v>16</v>
+      </c>
+      <c r="D119" t="s">
         <v>17</v>
-      </c>
-      <c r="D119" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2456,10 +2453,10 @@
         <v>5</v>
       </c>
       <c r="C120" t="s">
+        <v>16</v>
+      </c>
+      <c r="D120" t="s">
         <v>17</v>
-      </c>
-      <c r="D120" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2470,10 +2467,10 @@
         <v>5</v>
       </c>
       <c r="C121" t="s">
+        <v>16</v>
+      </c>
+      <c r="D121" t="s">
         <v>17</v>
-      </c>
-      <c r="D121" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2484,10 +2481,10 @@
         <v>5</v>
       </c>
       <c r="C122" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" t="s">
         <v>17</v>
-      </c>
-      <c r="D122" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2498,10 +2495,10 @@
         <v>5</v>
       </c>
       <c r="C123" t="s">
+        <v>16</v>
+      </c>
+      <c r="D123" t="s">
         <v>17</v>
-      </c>
-      <c r="D123" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2512,10 +2509,10 @@
         <v>5</v>
       </c>
       <c r="C124" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" t="s">
         <v>17</v>
-      </c>
-      <c r="D124" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2526,10 +2523,10 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" t="s">
         <v>17</v>
-      </c>
-      <c r="D125" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2540,10 +2537,10 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" t="s">
         <v>17</v>
-      </c>
-      <c r="D126" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2557,7 +2554,7 @@
         <v>11</v>
       </c>
       <c r="D127" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2565,13 +2562,13 @@
         <v>7015</v>
       </c>
       <c r="B128" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C128" t="s">
+        <v>19</v>
+      </c>
+      <c r="D128" t="s">
         <v>20</v>
-      </c>
-      <c r="D128" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2579,13 +2576,13 @@
         <v>7017</v>
       </c>
       <c r="B129" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
+        <v>19</v>
+      </c>
+      <c r="D129" t="s">
         <v>20</v>
-      </c>
-      <c r="D129" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2593,13 +2590,13 @@
         <v>7101</v>
       </c>
       <c r="B130" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C130" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" t="s">
         <v>20</v>
-      </c>
-      <c r="D130" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2607,13 +2604,13 @@
         <v>7102</v>
       </c>
       <c r="B131" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C131" t="s">
+        <v>19</v>
+      </c>
+      <c r="D131" t="s">
         <v>20</v>
-      </c>
-      <c r="D131" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2621,13 +2618,13 @@
         <v>7103</v>
       </c>
       <c r="B132" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C132" t="s">
+        <v>19</v>
+      </c>
+      <c r="D132" t="s">
         <v>20</v>
-      </c>
-      <c r="D132" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2635,13 +2632,13 @@
         <v>7104</v>
       </c>
       <c r="B133" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C133" t="s">
+        <v>19</v>
+      </c>
+      <c r="D133" t="s">
         <v>20</v>
-      </c>
-      <c r="D133" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2649,13 +2646,13 @@
         <v>7105</v>
       </c>
       <c r="B134" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C134" t="s">
+        <v>19</v>
+      </c>
+      <c r="D134" t="s">
         <v>20</v>
-      </c>
-      <c r="D134" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2663,13 +2660,13 @@
         <v>7106</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C135" t="s">
+        <v>19</v>
+      </c>
+      <c r="D135" t="s">
         <v>20</v>
-      </c>
-      <c r="D135" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2677,13 +2674,13 @@
         <v>7107</v>
       </c>
       <c r="B136" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C136" t="s">
+        <v>19</v>
+      </c>
+      <c r="D136" t="s">
         <v>20</v>
-      </c>
-      <c r="D136" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2691,13 +2688,13 @@
         <v>7108</v>
       </c>
       <c r="B137" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C137" t="s">
+        <v>19</v>
+      </c>
+      <c r="D137" t="s">
         <v>20</v>
-      </c>
-      <c r="D137" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2705,13 +2702,13 @@
         <v>7109</v>
       </c>
       <c r="B138" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C138" t="s">
+        <v>19</v>
+      </c>
+      <c r="D138" t="s">
         <v>20</v>
-      </c>
-      <c r="D138" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2719,13 +2716,13 @@
         <v>7110</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C139" t="s">
+        <v>19</v>
+      </c>
+      <c r="D139" t="s">
         <v>20</v>
-      </c>
-      <c r="D139" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2733,13 +2730,13 @@
         <v>7111</v>
       </c>
       <c r="B140" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C140" t="s">
+        <v>19</v>
+      </c>
+      <c r="D140" t="s">
         <v>20</v>
-      </c>
-      <c r="D140" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2747,13 +2744,13 @@
         <v>7112</v>
       </c>
       <c r="B141" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C141" t="s">
+        <v>19</v>
+      </c>
+      <c r="D141" t="s">
         <v>20</v>
-      </c>
-      <c r="D141" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2761,13 +2758,13 @@
         <v>7113</v>
       </c>
       <c r="B142" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C142" t="s">
+        <v>19</v>
+      </c>
+      <c r="D142" t="s">
         <v>20</v>
-      </c>
-      <c r="D142" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2775,13 +2772,13 @@
         <v>7114</v>
       </c>
       <c r="B143" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C143" t="s">
+        <v>19</v>
+      </c>
+      <c r="D143" t="s">
         <v>20</v>
-      </c>
-      <c r="D143" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2789,102 +2786,102 @@
         <v>7116</v>
       </c>
       <c r="B144" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C144" t="s">
+        <v>19</v>
+      </c>
+      <c r="D144" t="s">
         <v>20</v>
-      </c>
-      <c r="D144" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
+        <v>21</v>
+      </c>
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>16</v>
+      </c>
+      <c r="D145" t="s">
         <v>22</v>
-      </c>
-      <c r="B145" t="s">
-        <v>5</v>
-      </c>
-      <c r="C145" t="s">
-        <v>17</v>
-      </c>
-      <c r="D145" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
+        <v>23</v>
+      </c>
+      <c r="B146" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" t="s">
+        <v>16</v>
+      </c>
+      <c r="D146" t="s">
         <v>24</v>
-      </c>
-      <c r="B146" t="s">
-        <v>5</v>
-      </c>
-      <c r="C146" t="s">
-        <v>17</v>
-      </c>
-      <c r="D146" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
+        <v>25</v>
+      </c>
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>16</v>
+      </c>
+      <c r="D147" t="s">
         <v>26</v>
-      </c>
-      <c r="B147" t="s">
-        <v>5</v>
-      </c>
-      <c r="C147" t="s">
-        <v>17</v>
-      </c>
-      <c r="D147" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
+        <v>27</v>
+      </c>
+      <c r="B148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" t="s">
         <v>28</v>
       </c>
-      <c r="B148" t="s">
-        <v>13</v>
-      </c>
-      <c r="C148" t="s">
+      <c r="D148" t="s">
         <v>29</v>
-      </c>
-      <c r="D148" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B149" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C149" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D149" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
+        <v>31</v>
+      </c>
+      <c r="B150" t="s">
         <v>32</v>
       </c>
-      <c r="B150" t="s">
+      <c r="C150" t="s">
         <v>33</v>
       </c>
-      <c r="C150" t="s">
-        <v>34</v>
-      </c>
       <c r="D150" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B151" t="s">
         <v>5</v>
@@ -2893,12 +2890,12 @@
         <v>11</v>
       </c>
       <c r="D151" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B152" t="s">
         <v>5</v>
@@ -2907,40 +2904,40 @@
         <v>11</v>
       </c>
       <c r="D152" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
+        <v>37</v>
+      </c>
+      <c r="B153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153" t="s">
+        <v>13</v>
+      </c>
+      <c r="D153" t="s">
         <v>38</v>
-      </c>
-      <c r="B153" t="s">
-        <v>13</v>
-      </c>
-      <c r="C153" t="s">
-        <v>14</v>
-      </c>
-      <c r="D153" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B154" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" t="s">
         <v>13</v>
       </c>
-      <c r="C154" t="s">
-        <v>14</v>
-      </c>
       <c r="D154" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B155" t="s">
         <v>5</v>
@@ -2949,12 +2946,12 @@
         <v>6</v>
       </c>
       <c r="D155" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B156" t="s">
         <v>5</v>
@@ -2963,82 +2960,82 @@
         <v>6</v>
       </c>
       <c r="D156" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B157" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C157" t="s">
+        <v>19</v>
+      </c>
+      <c r="D157" t="s">
         <v>20</v>
-      </c>
-      <c r="D157" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B158" t="s">
         <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D158" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B159" t="s">
         <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D159" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
+        <v>47</v>
+      </c>
+      <c r="B160" t="s">
+        <v>5</v>
+      </c>
+      <c r="C160" t="s">
+        <v>16</v>
+      </c>
+      <c r="D160" t="s">
         <v>48</v>
-      </c>
-      <c r="B160" t="s">
-        <v>5</v>
-      </c>
-      <c r="C160" t="s">
-        <v>17</v>
-      </c>
-      <c r="D160" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D161" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B162" t="s">
         <v>5</v>
@@ -3047,502 +3044,502 @@
         <v>6</v>
       </c>
       <c r="D162" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B163" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C163" t="s">
+        <v>28</v>
+      </c>
+      <c r="D163" t="s">
         <v>29</v>
-      </c>
-      <c r="D163" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B164" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C164" t="s">
+        <v>28</v>
+      </c>
+      <c r="D164" t="s">
         <v>29</v>
-      </c>
-      <c r="D164" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
+        <v>54</v>
+      </c>
+      <c r="B165" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165" t="s">
+        <v>28</v>
+      </c>
+      <c r="D165" t="s">
         <v>55</v>
-      </c>
-      <c r="B165" t="s">
-        <v>13</v>
-      </c>
-      <c r="C165" t="s">
-        <v>29</v>
-      </c>
-      <c r="D165" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B166" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C166" t="s">
+        <v>28</v>
+      </c>
+      <c r="D166" t="s">
         <v>29</v>
-      </c>
-      <c r="D166" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
+        <v>57</v>
+      </c>
+      <c r="B167" t="s">
+        <v>32</v>
+      </c>
+      <c r="C167" t="s">
         <v>58</v>
       </c>
-      <c r="B167" t="s">
-        <v>33</v>
-      </c>
-      <c r="C167" t="s">
-        <v>59</v>
-      </c>
       <c r="D167" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B168" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C168" t="s">
+        <v>28</v>
+      </c>
+      <c r="D168" t="s">
         <v>29</v>
-      </c>
-      <c r="D168" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
+        <v>59</v>
+      </c>
+      <c r="B169" t="s">
         <v>60</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>61</v>
       </c>
-      <c r="C169" t="s">
+      <c r="D169" t="s">
         <v>62</v>
-      </c>
-      <c r="D169" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
+        <v>63</v>
+      </c>
+      <c r="B170" t="s">
         <v>64</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>65</v>
       </c>
-      <c r="C170" t="s">
+      <c r="D170" t="s">
         <v>66</v>
-      </c>
-      <c r="D170" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
+        <v>67</v>
+      </c>
+      <c r="B171" t="s">
+        <v>64</v>
+      </c>
+      <c r="C171" t="s">
+        <v>65</v>
+      </c>
+      <c r="D171" t="s">
         <v>68</v>
-      </c>
-      <c r="B171" t="s">
-        <v>65</v>
-      </c>
-      <c r="C171" t="s">
-        <v>66</v>
-      </c>
-      <c r="D171" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B172" t="s">
+        <v>64</v>
+      </c>
+      <c r="C172" t="s">
         <v>65</v>
       </c>
-      <c r="C172" t="s">
+      <c r="D172" t="s">
         <v>66</v>
-      </c>
-      <c r="D172" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B173" t="s">
+        <v>64</v>
+      </c>
+      <c r="C173" t="s">
         <v>65</v>
       </c>
-      <c r="C173" t="s">
+      <c r="D173" t="s">
         <v>66</v>
-      </c>
-      <c r="D173" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
+        <v>71</v>
+      </c>
+      <c r="B174" t="s">
+        <v>64</v>
+      </c>
+      <c r="C174" t="s">
+        <v>65</v>
+      </c>
+      <c r="D174" t="s">
         <v>72</v>
-      </c>
-      <c r="B174" t="s">
-        <v>65</v>
-      </c>
-      <c r="C174" t="s">
-        <v>66</v>
-      </c>
-      <c r="D174" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B175" t="s">
+        <v>64</v>
+      </c>
+      <c r="C175" t="s">
         <v>65</v>
       </c>
-      <c r="C175" t="s">
-        <v>66</v>
-      </c>
       <c r="D175" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B176" t="s">
+        <v>64</v>
+      </c>
+      <c r="C176" t="s">
         <v>65</v>
       </c>
-      <c r="C176" t="s">
-        <v>66</v>
-      </c>
       <c r="D176" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B177" t="s">
+        <v>64</v>
+      </c>
+      <c r="C177" t="s">
         <v>65</v>
       </c>
-      <c r="C177" t="s">
+      <c r="D177" t="s">
         <v>66</v>
-      </c>
-      <c r="D177" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B178" t="s">
+        <v>64</v>
+      </c>
+      <c r="C178" t="s">
         <v>65</v>
       </c>
-      <c r="C178" t="s">
-        <v>66</v>
-      </c>
       <c r="D178" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B179" t="s">
+        <v>64</v>
+      </c>
+      <c r="C179" t="s">
         <v>65</v>
       </c>
-      <c r="C179" t="s">
+      <c r="D179" t="s">
         <v>66</v>
-      </c>
-      <c r="D179" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B180" t="s">
+        <v>64</v>
+      </c>
+      <c r="C180" t="s">
         <v>65</v>
       </c>
-      <c r="C180" t="s">
+      <c r="D180" t="s">
         <v>66</v>
-      </c>
-      <c r="D180" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B181" t="s">
+        <v>64</v>
+      </c>
+      <c r="C181" t="s">
         <v>65</v>
       </c>
-      <c r="C181" t="s">
-        <v>66</v>
-      </c>
       <c r="D181" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B182" t="s">
+        <v>64</v>
+      </c>
+      <c r="C182" t="s">
         <v>65</v>
       </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>66</v>
-      </c>
-      <c r="D182" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
+        <v>81</v>
+      </c>
+      <c r="B183" t="s">
+        <v>64</v>
+      </c>
+      <c r="C183" t="s">
+        <v>65</v>
+      </c>
+      <c r="D183" t="s">
         <v>82</v>
-      </c>
-      <c r="B183" t="s">
-        <v>65</v>
-      </c>
-      <c r="C183" t="s">
-        <v>66</v>
-      </c>
-      <c r="D183" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B184" t="s">
+        <v>64</v>
+      </c>
+      <c r="C184" t="s">
         <v>65</v>
       </c>
-      <c r="C184" t="s">
-        <v>66</v>
-      </c>
       <c r="D184" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B185" t="s">
+        <v>64</v>
+      </c>
+      <c r="C185" t="s">
         <v>65</v>
       </c>
-      <c r="C185" t="s">
+      <c r="D185" t="s">
         <v>66</v>
-      </c>
-      <c r="D185" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B186" t="s">
+        <v>64</v>
+      </c>
+      <c r="C186" t="s">
         <v>65</v>
       </c>
-      <c r="C186" t="s">
+      <c r="D186" t="s">
         <v>66</v>
-      </c>
-      <c r="D186" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B187" t="s">
+        <v>64</v>
+      </c>
+      <c r="C187" t="s">
         <v>65</v>
       </c>
-      <c r="C187" t="s">
+      <c r="D187" t="s">
         <v>66</v>
-      </c>
-      <c r="D187" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B188" t="s">
+        <v>64</v>
+      </c>
+      <c r="C188" t="s">
         <v>65</v>
       </c>
-      <c r="C188" t="s">
-        <v>66</v>
-      </c>
       <c r="D188" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B189" t="s">
+        <v>64</v>
+      </c>
+      <c r="C189" t="s">
         <v>65</v>
       </c>
-      <c r="C189" t="s">
-        <v>66</v>
-      </c>
       <c r="D189" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B190" t="s">
+        <v>64</v>
+      </c>
+      <c r="C190" t="s">
         <v>65</v>
       </c>
-      <c r="C190" t="s">
-        <v>66</v>
-      </c>
       <c r="D190" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B191" t="s">
+        <v>64</v>
+      </c>
+      <c r="C191" t="s">
         <v>65</v>
       </c>
-      <c r="C191" t="s">
-        <v>66</v>
-      </c>
       <c r="D191" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B192" t="s">
+        <v>64</v>
+      </c>
+      <c r="C192" t="s">
         <v>65</v>
       </c>
-      <c r="C192" t="s">
+      <c r="D192" t="s">
         <v>66</v>
-      </c>
-      <c r="D192" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B193" t="s">
+        <v>64</v>
+      </c>
+      <c r="C193" t="s">
         <v>65</v>
       </c>
-      <c r="C193" t="s">
+      <c r="D193" t="s">
         <v>66</v>
-      </c>
-      <c r="D193" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
+        <v>93</v>
+      </c>
+      <c r="B194" t="s">
+        <v>64</v>
+      </c>
+      <c r="C194" t="s">
         <v>94</v>
       </c>
-      <c r="B194" t="s">
-        <v>65</v>
-      </c>
-      <c r="C194" t="s">
+      <c r="D194" t="s">
         <v>95</v>
-      </c>
-      <c r="D194" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
+        <v>96</v>
+      </c>
+      <c r="B195" t="s">
+        <v>64</v>
+      </c>
+      <c r="C195" t="s">
+        <v>94</v>
+      </c>
+      <c r="D195" t="s">
         <v>97</v>
-      </c>
-      <c r="B195" t="s">
-        <v>65</v>
-      </c>
-      <c r="C195" t="s">
-        <v>95</v>
-      </c>
-      <c r="D195" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
+        <v>98</v>
+      </c>
+      <c r="B196" t="s">
+        <v>64</v>
+      </c>
+      <c r="C196" t="s">
+        <v>94</v>
+      </c>
+      <c r="D196" t="s">
         <v>99</v>
-      </c>
-      <c r="B196" t="s">
-        <v>65</v>
-      </c>
-      <c r="C196" t="s">
-        <v>95</v>
-      </c>
-      <c r="D196" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B197" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C197" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D197" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B198" t="s">
         <v>5</v>
@@ -3551,12 +3548,12 @@
         <v>11</v>
       </c>
       <c r="D198" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B199" t="s">
         <v>5</v>
@@ -3565,40 +3562,40 @@
         <v>11</v>
       </c>
       <c r="D199" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B200" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200" t="s">
         <v>13</v>
       </c>
-      <c r="C200" t="s">
-        <v>14</v>
-      </c>
       <c r="D200" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B201" t="s">
+        <v>5</v>
+      </c>
+      <c r="C201" t="s">
         <v>13</v>
       </c>
-      <c r="C201" t="s">
-        <v>14</v>
-      </c>
       <c r="D201" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B202" t="s">
         <v>5</v>
@@ -3607,12 +3604,12 @@
         <v>6</v>
       </c>
       <c r="D202" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B203" t="s">
         <v>5</v>
@@ -3621,68 +3618,68 @@
         <v>6</v>
       </c>
       <c r="D203" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
+        <v>107</v>
+      </c>
+      <c r="B204" t="s">
+        <v>5</v>
+      </c>
+      <c r="C204" t="s">
+        <v>19</v>
+      </c>
+      <c r="D204" t="s">
         <v>108</v>
-      </c>
-      <c r="B204" t="s">
-        <v>13</v>
-      </c>
-      <c r="C204" t="s">
-        <v>20</v>
-      </c>
-      <c r="D204" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B205" t="s">
         <v>5</v>
       </c>
       <c r="C205" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D205" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B206" t="s">
         <v>5</v>
       </c>
       <c r="C206" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D206" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B207" t="s">
         <v>5</v>
       </c>
       <c r="C207" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D207" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B208" t="s">
         <v>5</v>
@@ -3691,161 +3688,161 @@
         <v>6</v>
       </c>
       <c r="D208" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B209" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C209" t="s">
+        <v>28</v>
+      </c>
+      <c r="D209" t="s">
         <v>29</v>
-      </c>
-      <c r="D209" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B210" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C210" t="s">
+        <v>28</v>
+      </c>
+      <c r="D210" t="s">
         <v>29</v>
-      </c>
-      <c r="D210" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B211" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D211" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B212" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C212" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D212" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B213" t="s">
+        <v>60</v>
+      </c>
+      <c r="C213" t="s">
         <v>61</v>
       </c>
-      <c r="C213" t="s">
+      <c r="D213" t="s">
         <v>62</v>
-      </c>
-      <c r="D213" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B214" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C214" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D214" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B215" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C215" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D215" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B216" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C216" t="s">
+        <v>28</v>
+      </c>
+      <c r="D216" t="s">
         <v>29</v>
-      </c>
-      <c r="D216" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B217" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C217" t="s">
+        <v>28</v>
+      </c>
+      <c r="D217" t="s">
         <v>29</v>
-      </c>
-      <c r="D217" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B218" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C218" t="s">
+        <v>28</v>
+      </c>
+      <c r="D218" t="s">
         <v>29</v>
-      </c>
-      <c r="D218" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B219" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C219" t="s">
+        <v>28</v>
+      </c>
+      <c r="D219" t="s">
         <v>29</v>
-      </c>
-      <c r="D219" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3967,6 +3964,18 @@
       <c r="B239"/>
       <c r="C239"/>
       <c r="D239"/>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240"/>
+      <c r="B240"/>
+      <c r="C240"/>
+      <c r="D240"/>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241"/>
+      <c r="B241"/>
+      <c r="C241"/>
+      <c r="D241"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
UPDATED SAS FNCTION FOR USER_DEPARTMENT
</commit_message>
<xml_diff>
--- a/functions/templates/Line Transfer.xlsx
+++ b/functions/templates/Line Transfer.xlsx
@@ -764,7 +764,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D244"/>
+  <dimension ref="A1:D245"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A155" sqref="A155"/>
@@ -3991,6 +3991,12 @@
       <c r="B244"/>
       <c r="C244"/>
       <c r="D244"/>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245"/>
+      <c r="B245"/>
+      <c r="C245"/>
+      <c r="D245"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>